<commit_message>
created some pages for Admin
</commit_message>
<xml_diff>
--- a/Documentation/DB Design/DB tables and queries V 0.2.xlsx
+++ b/Documentation/DB Design/DB tables and queries V 0.2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
   <si>
     <t>TABLES</t>
   </si>
@@ -129,15 +129,6 @@
     <t>className</t>
   </si>
   <si>
-    <t>DevisionMaster</t>
-  </si>
-  <si>
-    <t>DevisionId</t>
-  </si>
-  <si>
-    <t>DevisionName</t>
-  </si>
-  <si>
     <t>BatchMaster</t>
   </si>
   <si>
@@ -268,6 +259,18 @@
   </si>
   <si>
     <t>Also some tables are newly added.</t>
+  </si>
+  <si>
+    <t>DivisionMaster</t>
+  </si>
+  <si>
+    <t>DivisionId</t>
+  </si>
+  <si>
+    <t>DivisionName</t>
+  </si>
+  <si>
+    <t>Member table</t>
   </si>
 </sst>
 </file>
@@ -389,38 +392,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -428,6 +401,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,15 +796,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.28515625"/>
     <col min="2" max="2" width="31.140625"/>
-    <col min="3" max="3" width="1.28515625" style="13"/>
+    <col min="3" max="3" width="1.28515625" style="1"/>
     <col min="4" max="4" width="14.140625"/>
     <col min="5" max="5" width="5.5703125"/>
     <col min="6" max="6" width="173.140625"/>
@@ -813,740 +817,740 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10">
+      <c r="A3" s="12">
         <v>43480</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="8"/>
+      <c r="D5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="14" t="s">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="6"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="14" t="s">
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="11"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="6" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="11"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="14" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="11"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B60" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="12">
+        <v>43486</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="D70" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="6"/>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="6" t="s">
+    <row r="74" spans="1:6">
+      <c r="A74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" s="11"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="14" t="s">
+      <c r="B84" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B89" s="7"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="8"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B102" s="8"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="6"/>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="6"/>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="10">
-        <v>43486</v>
-      </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="9"/>
-      <c r="D70" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B82" s="6"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B89" s="4"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="9" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B94" s="9"/>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="14" t="s">
+      <c r="B106" s="9"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B97" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="9" t="s">
+      <c r="B107" s="10"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B102" s="9"/>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B104" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B108" s="1"/>
+      <c r="B108" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="A82:B82"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added hide & show facility to createAcc.html
</commit_message>
<xml_diff>
--- a/Documentation/DB Design/DB tables and queries V 0.2.xlsx
+++ b/Documentation/DB Design/DB tables and queries V 0.2.xlsx
@@ -401,37 +401,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -817,36 +817,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>43480</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="10"/>
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
@@ -855,7 +855,7 @@
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -872,7 +872,7 @@
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
@@ -937,10 +937,10 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
@@ -991,10 +991,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
@@ -1013,13 +1013,13 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1027,7 +1027,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1035,10 +1035,10 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="11"/>
+      <c r="B39" s="13"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
@@ -1103,10 +1103,10 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="13"/>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
@@ -1133,10 +1133,10 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="11"/>
+      <c r="B48" s="13"/>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
@@ -1155,10 +1155,10 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="11"/>
+      <c r="B52" s="13"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
@@ -1193,10 +1193,10 @@
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="11"/>
+      <c r="B58" s="13"/>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
@@ -1231,10 +1231,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="11"/>
+      <c r="B64" s="13"/>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
@@ -1253,25 +1253,25 @@
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="12">
+      <c r="A68" s="9">
         <v>43486</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="8"/>
-      <c r="D70" s="13" t="s">
+      <c r="B70" s="10"/>
+      <c r="D70" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
@@ -1354,10 +1354,10 @@
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="11"/>
+      <c r="B82" s="13"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2" t="s">
@@ -1400,10 +1400,10 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B89" s="7"/>
+      <c r="B89" s="16"/>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2" t="s">
@@ -1430,10 +1430,10 @@
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="8"/>
+      <c r="B94" s="10"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2" t="s">
@@ -1484,10 +1484,10 @@
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="8" t="s">
+      <c r="A102" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B102" s="8"/>
+      <c r="B102" s="10"/>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2" t="s">
@@ -1506,51 +1506,51 @@
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B106" s="9"/>
+      <c r="B106" s="17"/>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B107" s="10"/>
+      <c r="B107" s="18"/>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B108" s="6"/>
+      <c r="B108" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="A82:B82"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>